<commit_message>
oops session 7 revised
</commit_message>
<xml_diff>
--- a/Courses Offered.xlsx
+++ b/Courses Offered.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19485" windowHeight="7800" activeTab="1"/>
+    <workbookView windowWidth="19395" windowHeight="7800" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="57">
   <si>
     <t>SL No</t>
   </si>
@@ -186,16 +186,6 @@
   </si>
   <si>
     <t>SL NO</t>
-  </si>
-  <si>
-    <t>OS Concepts : Linux Commands, Vi editor, Shell Scripting, Overview of OS, Processes, Scheduling &amp; Synchronization, Memory management, File Systems, Case Study with Linux System Programming: Process, Signals, Semaphores &amp; Mutex, Inter – Process Communication, POSIX Threads</t>
-  </si>
-  <si>
-    <t>Database Concepts: Client/Server Computing,RDBMS Technologies,Codd’s Rules,Data Models,Normalization Techniques,ER Diagrams,
-SQL : Overview of OORD,Introduction SQL*Plus,DDL, DML and DCL,Tables, Indexes and Views,Clusters, Sequences and Snapshots,Cursors,Stored Procedures, Triggers, Packages, Introduction to No SQL, MongoDB (Virtual DB)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Client/Server Computing,RDBMS Technologies,Codd’s Rules,Data Models,Normalization Techniques,ER Diagrams,</t>
   </si>
 </sst>
 </file>
@@ -203,9 +193,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
@@ -217,39 +207,37 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -263,6 +251,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -270,16 +275,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -295,15 +307,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -311,22 +315,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -339,13 +335,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -354,10 +344,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -370,31 +360,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -406,151 +534,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -580,25 +570,31 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -614,21 +610,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -656,23 +637,32 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -681,152 +671,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -835,9 +825,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1194,10 +1181,10 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1205,66 +1192,66 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
       <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
       <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
       <c r="C7" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
       <c r="C8" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
       <c r="C9" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
       <c r="C10" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="5">
+      <c r="A11" s="4">
         <v>2</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1272,52 +1259,52 @@
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
       <c r="C12" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
       <c r="C13" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
       <c r="C14" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
       <c r="C15" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
       <c r="C16" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
       <c r="C17" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="5">
+      <c r="A18" s="4">
         <v>3</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -1325,59 +1312,59 @@
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
       <c r="C19" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
       <c r="C20" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
       <c r="C21" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
       <c r="C22" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
       <c r="C23" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
       <c r="C24" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
       <c r="C25" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="5">
+      <c r="A26" s="4">
         <v>4</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C26" s="2" t="s">
@@ -1385,52 +1372,52 @@
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
       <c r="C27" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
       <c r="C28" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
       <c r="C29" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
       <c r="C30" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
       <c r="C31" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
       <c r="C32" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="5">
+      <c r="A33" s="4">
         <v>5</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C33" s="2" t="s">
@@ -1438,45 +1425,45 @@
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
       <c r="C34" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
       <c r="C35" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
       <c r="C36" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
       <c r="C37" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="5"/>
-      <c r="B38" s="5"/>
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
       <c r="C38" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="5">
+      <c r="A39" s="4">
         <v>6</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C39" s="2" t="s">
@@ -1484,38 +1471,38 @@
       </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
       <c r="C40" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
       <c r="C41" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
       <c r="C42" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="6"/>
-      <c r="B43" s="5"/>
+      <c r="A43" s="5"/>
+      <c r="B43" s="4"/>
       <c r="C43" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="5">
+      <c r="A44" s="4">
         <v>7</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C44" s="2" t="s">
@@ -1523,38 +1510,38 @@
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
       <c r="C45" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="5"/>
-      <c r="B46" s="5"/>
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
       <c r="C46" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5"/>
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
       <c r="C47" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
       <c r="C48" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="5">
+      <c r="A49" s="4">
         <v>8</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="4" t="s">
         <v>39</v>
       </c>
       <c r="C49" s="2" t="s">
@@ -1562,31 +1549,31 @@
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5"/>
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
       <c r="C50" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="5"/>
-      <c r="B51" s="5"/>
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
       <c r="C51" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="5"/>
-      <c r="B52" s="5"/>
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
       <c r="C52" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="5">
+      <c r="A53" s="4">
         <v>9</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="B53" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C53" s="2" t="s">
@@ -1594,38 +1581,38 @@
       </c>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="5"/>
-      <c r="B54" s="5"/>
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
       <c r="C54" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" s="5"/>
-      <c r="B55" s="5"/>
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
       <c r="C55" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="56" spans="1:3">
-      <c r="A56" s="5"/>
-      <c r="B56" s="5"/>
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
       <c r="C56" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="57" spans="1:3">
-      <c r="A57" s="5"/>
-      <c r="B57" s="5"/>
+      <c r="A57" s="4"/>
+      <c r="B57" s="4"/>
       <c r="C57" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="58" spans="1:3">
-      <c r="A58" s="5">
+      <c r="A58" s="4">
         <v>10</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B58" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C58" s="2" t="s">
@@ -1633,45 +1620,45 @@
       </c>
     </row>
     <row r="59" spans="1:3">
-      <c r="A59" s="5"/>
-      <c r="B59" s="5"/>
+      <c r="A59" s="4"/>
+      <c r="B59" s="4"/>
       <c r="C59" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" s="5"/>
-      <c r="B60" s="5"/>
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
       <c r="C60" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" s="5"/>
-      <c r="B61" s="5"/>
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
       <c r="C61" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="62" spans="1:3">
-      <c r="A62" s="5"/>
-      <c r="B62" s="5"/>
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
       <c r="C62" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="63" spans="1:3">
-      <c r="A63" s="5"/>
-      <c r="B63" s="5"/>
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
       <c r="C63" s="2" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="64" spans="1:3">
-      <c r="A64" s="5">
+      <c r="A64" s="4">
         <v>11</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" s="4" t="s">
         <v>55</v>
       </c>
       <c r="C64" s="2" t="s">
@@ -1679,87 +1666,87 @@
       </c>
     </row>
     <row r="65" spans="1:3">
-      <c r="A65" s="5"/>
-      <c r="B65" s="5"/>
+      <c r="A65" s="4"/>
+      <c r="B65" s="4"/>
       <c r="C65" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:3">
-      <c r="A66" s="5"/>
-      <c r="B66" s="5"/>
+      <c r="A66" s="4"/>
+      <c r="B66" s="4"/>
       <c r="C66" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="67" spans="1:3">
-      <c r="A67" s="5"/>
-      <c r="B67" s="5"/>
+      <c r="A67" s="4"/>
+      <c r="B67" s="4"/>
       <c r="C67" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="68" spans="1:3">
-      <c r="A68" s="5"/>
-      <c r="B68" s="5"/>
+      <c r="A68" s="4"/>
+      <c r="B68" s="4"/>
       <c r="C68" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="69" spans="1:3">
-      <c r="A69" s="5"/>
-      <c r="B69" s="5"/>
+      <c r="A69" s="4"/>
+      <c r="B69" s="4"/>
       <c r="C69" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" s="5"/>
-      <c r="B70" s="5"/>
+      <c r="A70" s="4"/>
+      <c r="B70" s="4"/>
       <c r="C70" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="71" spans="1:3">
-      <c r="A71" s="5"/>
-      <c r="B71" s="5"/>
+      <c r="A71" s="4"/>
+      <c r="B71" s="4"/>
       <c r="C71" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="72" spans="1:3">
-      <c r="A72" s="5"/>
-      <c r="B72" s="5"/>
+      <c r="A72" s="4"/>
+      <c r="B72" s="4"/>
       <c r="C72" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="73" spans="1:1">
-      <c r="A73" s="7"/>
+      <c r="A73" s="6"/>
     </row>
     <row r="74" spans="1:1">
-      <c r="A74" s="7"/>
+      <c r="A74" s="6"/>
     </row>
     <row r="75" spans="1:1">
-      <c r="A75" s="7"/>
+      <c r="A75" s="6"/>
     </row>
     <row r="76" spans="1:1">
-      <c r="A76" s="7"/>
+      <c r="A76" s="6"/>
     </row>
     <row r="77" spans="1:1">
-      <c r="A77" s="7"/>
+      <c r="A77" s="6"/>
     </row>
     <row r="78" spans="1:1">
-      <c r="A78" s="7"/>
+      <c r="A78" s="6"/>
     </row>
     <row r="79" spans="1:1">
-      <c r="A79" s="7"/>
+      <c r="A79" s="6"/>
     </row>
     <row r="80" spans="1:1">
-      <c r="A80" s="7"/>
+      <c r="A80" s="6"/>
     </row>
     <row r="81" spans="1:1">
-      <c r="A81" s="7"/>
+      <c r="A81" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="22">
@@ -1797,7 +1784,7 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75" outlineLevelCol="2"/>
@@ -1815,16 +1802,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" ht="63" spans="1:3">
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>57</v>
-      </c>
+      <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1">
@@ -1858,16 +1843,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" ht="94.5" spans="1:3">
+    <row r="7" spans="1:3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>58</v>
-      </c>
+      <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1">
@@ -1909,16 +1892,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" ht="31.5" spans="1:3">
+    <row r="13" spans="1:3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>59</v>
-      </c>
+      <c r="C13" s="3"/>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1">

</xml_diff>